<commit_message>
started on pivot tables
</commit_message>
<xml_diff>
--- a/Lineups/lineup_survey_results.xlsx
+++ b/Lineups/lineup_survey_results.xlsx
@@ -1,22 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27126"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/s1941220_ed_ac_uk/Documents/Year 5/Dissertation/Code/MMath_Y5_Dissertation/Lineups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="13_ncr:1_{AD74628D-BE06-4FC1-BE04-2187DD70E9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7420FE8-E67C-4657-97F5-1A5EB4F0989B}"/>
+  <xr:revisionPtr revIDLastSave="65" documentId="13_ncr:1_{AD74628D-BE06-4FC1-BE04-2187DD70E9AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{881B352B-56C4-4DD8-8B8E-0BC8478FCA9B}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="cleaned_data" sheetId="1" r:id="rId1"/>
     <sheet name="full_data" sheetId="2" r:id="rId2"/>
+    <sheet name="Tables" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <pivotCaches>
+    <pivotCache cacheId="6" r:id="rId4"/>
+  </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2382" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2395" uniqueCount="251">
   <si>
     <t>ID</t>
   </si>
@@ -779,6 +783,15 @@
   </si>
   <si>
     <t>LU8_comments</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Count of Stats Y2</t>
   </si>
 </sst>
 </file>
@@ -786,7 +799,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -823,12 +836,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -919,7 +940,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -928,34 +949,19 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="m/d/yy\ h:mm:ss"/>
+      <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm:ss"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="1" formatCode="0"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="1" formatCode="0"/>
@@ -967,7 +973,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -976,7 +982,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -985,7 +991,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -994,7 +1000,7 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1003,10 +1009,25 @@
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -1030,6 +1051,1883 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshedBy="Mayez Haris" refreshedDate="45313.539649999999" createdVersion="8" refreshedVersion="8" minRefreshableVersion="3" recordCount="57" xr:uid="{9800BCAF-FC90-4A1F-B493-74E2406460E2}">
+  <cacheSource type="worksheet">
+    <worksheetSource name="Table1"/>
+  </cacheSource>
+  <cacheFields count="27">
+    <cacheField name="Stats Y2" numFmtId="0">
+      <sharedItems count="2">
+        <s v="Yes"/>
+        <s v="No"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Level of study" numFmtId="0">
+      <sharedItems count="2">
+        <s v="Undergraduate"/>
+        <s v="Postgraduate"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Year of study" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="LU1" numFmtId="1">
+      <sharedItems count="3">
+        <s v="8"/>
+        <s v="3"/>
+        <s v="7"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="LU1_confidence" numFmtId="0">
+      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+    </cacheField>
+    <cacheField name="LU1_comments" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="LU2" numFmtId="1">
+      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="0"/>
+    </cacheField>
+    <cacheField name="LU2_confidence" numFmtId="0">
+      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+    </cacheField>
+    <cacheField name="LU2_comments" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="LU3" numFmtId="1">
+      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="0"/>
+    </cacheField>
+    <cacheField name="LU3_confidence" numFmtId="0">
+      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+    </cacheField>
+    <cacheField name="LU3_comments" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="LU4" numFmtId="1">
+      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="0"/>
+    </cacheField>
+    <cacheField name="LU4_confidence" numFmtId="0">
+      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+    </cacheField>
+    <cacheField name="LU4_comments" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="LU5" numFmtId="1">
+      <sharedItems count="2">
+        <s v="7"/>
+        <s v="5"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="LU5_confidence" numFmtId="0">
+      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+    </cacheField>
+    <cacheField name="LU5_comments" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="LU6" numFmtId="1">
+      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="0"/>
+    </cacheField>
+    <cacheField name="LU6_confidence" numFmtId="0">
+      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+    </cacheField>
+    <cacheField name="LU6_comments" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="LU7" numFmtId="1">
+      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="0"/>
+    </cacheField>
+    <cacheField name="LU7_confidence" numFmtId="0">
+      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+    </cacheField>
+    <cacheField name="LU7_comments" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+    <cacheField name="LU8" numFmtId="1">
+      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="0"/>
+    </cacheField>
+    <cacheField name="LU8_confidence" numFmtId="0">
+      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="1" maxValue="5"/>
+    </cacheField>
+    <cacheField name="LU8_comments" numFmtId="0">
+      <sharedItems containsBlank="1"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="57">
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 5"/>
+    <x v="0"/>
+    <s v="4"/>
+    <s v="It looks parabolic, whilst the others seem more linear"/>
+    <s v="9"/>
+    <s v="4"/>
+    <s v="Similar to the previous one; 9 has no clear linear form, while the others at least try."/>
+    <n v="0"/>
+    <s v="2"/>
+    <s v="They all seem to have different types of random noise, all contributing to things being fairly similar looking"/>
+    <n v="0"/>
+    <n v="1"/>
+    <s v="Things seem clustered in the same way, with enough different sorts of random noise to still seem the same."/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="Very clearly for 7, different lines that I choose will have a different distribution of points. "/>
+    <s v="5"/>
+    <s v="3"/>
+    <s v="Has got a very distinct shape for the rest of them, that can't be simply chalked up to outliers messing with the data"/>
+    <s v="6"/>
+    <s v="3"/>
+    <s v="I feel it's either 6, or they're all the same. The upward trajectory towards the tail end of 6 is throwing me a bit, hence telling me it should probably the one that's slightly different."/>
+    <n v="0"/>
+    <s v="2"/>
+    <s v="Tougher to see without the red line, but they do seem to be randomly distributed from the same guy"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="Year 5"/>
+    <x v="0"/>
+    <s v="4"/>
+    <s v="It looks parabolic while the others look straight"/>
+    <s v="9"/>
+    <s v="4"/>
+    <s v="Each of the others curve into directions (at least a little) while 9 only curves in one. "/>
+    <n v="0"/>
+    <s v="3"/>
+    <s v="They seem to have similar random noise and similar fittings."/>
+    <s v="2"/>
+    <s v="2"/>
+    <s v="2 has by eye a more significant portion of the data points below the dotted line, but they all look to be pretty similar."/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="The others all look close to straight with some variation, but in 7 there is a clear trend."/>
+    <s v="5"/>
+    <s v="3"/>
+    <s v="5 has the most what I can only describe as &quot;dramatic&quot; curve compared to the others."/>
+    <s v="6"/>
+    <s v="3"/>
+    <s v="The red line in the plot of 6 is noticeably steeper than the others. "/>
+    <s v="5"/>
+    <s v="2"/>
+    <s v="The points at height 1.5 are more spread out than in the other plots."/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 4"/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="Quadratic fit line, points higher up on the extremes compared to middle values"/>
+    <s v="9"/>
+    <n v="5"/>
+    <s v="Sharpest angle change in fit line"/>
+    <s v="6"/>
+    <s v="4"/>
+    <s v="After the bunch of points on the left side, it is the only line which jumps above the x axis which then crosses down under the x axis"/>
+    <s v="2"/>
+    <s v="2"/>
+    <s v="On the left of the plot, the points seem to all be below the x axis whereas the other plots have some above and below"/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="Clearest non constant variance as the points at the extremes are far above the x axis"/>
+    <s v="5"/>
+    <s v="3"/>
+    <s v="The plots all look similar towards the middle so this plot looked the most different to the others at the extremes"/>
+    <n v="0"/>
+    <s v="2"/>
+    <m/>
+    <n v="0"/>
+    <s v="4"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 4"/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v=":)"/>
+    <s v="9"/>
+    <s v="4"/>
+    <s v=":("/>
+    <n v="0"/>
+    <s v="4"/>
+    <m/>
+    <s v="2"/>
+    <s v="4"/>
+    <s v=":("/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v=":3"/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+    <n v="0"/>
+    <s v="4"/>
+    <m/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 4"/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="The red line is very bendy compared to the others"/>
+    <s v="9"/>
+    <n v="5"/>
+    <s v="The red line is very bendy"/>
+    <s v="6"/>
+    <s v="4"/>
+    <s v="The red line moves away from the centre line in the middle, rather than the tail end"/>
+    <n v="0"/>
+    <n v="1"/>
+    <s v="They all have similar distributions"/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="Very bendy red line"/>
+    <s v="2"/>
+    <s v="4"/>
+    <m/>
+    <s v="6"/>
+    <s v="4"/>
+    <m/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 4"/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="negative x values are more positive"/>
+    <s v="9"/>
+    <s v="4"/>
+    <m/>
+    <s v="6"/>
+    <s v="3"/>
+    <s v="weird red line"/>
+    <s v="2"/>
+    <s v="3"/>
+    <s v="higher central mass at x=0"/>
+    <x v="0"/>
+    <s v="4"/>
+    <s v="higher positive points at at extreme x values"/>
+    <s v="9"/>
+    <s v="2"/>
+    <s v="not as densely packed_x000a_"/>
+    <s v="9"/>
+    <n v="1"/>
+    <s v="least densely packed"/>
+    <s v="8"/>
+    <n v="1"/>
+    <s v="least densely packed in the bottom centre blob"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 5"/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="smiley :)"/>
+    <s v="9"/>
+    <s v="3"/>
+    <s v="frowny"/>
+    <s v="6"/>
+    <s v="2"/>
+    <s v="diverges and spends the most time away from the red line"/>
+    <s v="1"/>
+    <n v="1"/>
+    <s v="more noise"/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="big trough"/>
+    <s v="5"/>
+    <s v="3"/>
+    <s v="moves drastically away at both start and end"/>
+    <s v="3"/>
+    <n v="1"/>
+    <s v="more spread out"/>
+    <s v="5"/>
+    <n v="1"/>
+    <s v="concentrated top line"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 4"/>
+    <x v="0"/>
+    <s v="4"/>
+    <s v="8 is the only plot which resembles a parabola."/>
+    <s v="9"/>
+    <s v="4"/>
+    <s v="9 is, again, the only one that is a parabola. Other look more linear."/>
+    <n v="0"/>
+    <s v="2"/>
+    <s v="They all look the same (they cluster at one spot)."/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+    <x v="0"/>
+    <s v="4"/>
+    <s v="The other resemble a line more."/>
+    <s v="5"/>
+    <s v="2"/>
+    <s v="5 is the curviest."/>
+    <s v="6"/>
+    <s v="3"/>
+    <s v="6 curves upwards the most"/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 5"/>
+    <x v="0"/>
+    <s v="4"/>
+    <s v="The large deviations at each tail"/>
+    <s v="9"/>
+    <s v="4"/>
+    <s v="Large deviations at each tail"/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+    <s v="8"/>
+    <s v="2"/>
+    <s v="low residuals at each tail"/>
+    <x v="0"/>
+    <s v="4"/>
+    <s v="uptrends in residual sizes at tails"/>
+    <n v="0"/>
+    <s v="2"/>
+    <m/>
+    <n v="0"/>
+    <s v="4"/>
+    <m/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 3"/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="Its significantly curved."/>
+    <s v="9"/>
+    <s v="4"/>
+    <s v="Its curved unlike any other."/>
+    <s v="5"/>
+    <s v="2"/>
+    <s v="It's the least straight where there is a large concentration of data."/>
+    <s v="2"/>
+    <n v="1"/>
+    <s v="The data curved downward on the right, unlike the other plots where it more or less condenses on the axis."/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="It is W-shaped."/>
+    <n v="0"/>
+    <s v="4"/>
+    <s v="n/a"/>
+    <s v="6"/>
+    <n v="1"/>
+    <s v="Goes completely up on the right, may not be significant as it relies on a few points."/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 4"/>
+    <x v="0"/>
+    <s v="4"/>
+    <s v="All the others are distributed around a straight line, but 8 are distributed round a curve"/>
+    <s v="9"/>
+    <s v="4"/>
+    <s v="It has the most significant deviation"/>
+    <s v="6"/>
+    <s v="3"/>
+    <m/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+    <x v="0"/>
+    <s v="4"/>
+    <s v="W shape"/>
+    <s v="2"/>
+    <s v="2"/>
+    <m/>
+    <s v="6"/>
+    <s v="4"/>
+    <m/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 3"/>
+    <x v="0"/>
+    <s v="4"/>
+    <m/>
+    <s v="9"/>
+    <s v="4"/>
+    <m/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+    <x v="0"/>
+    <s v="4"/>
+    <m/>
+    <n v="0"/>
+    <s v="4"/>
+    <m/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+    <n v="0"/>
+    <s v="4"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 4"/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="It tapers off on both ends of the graph creating a curve for the line of best fit "/>
+    <s v="9"/>
+    <n v="5"/>
+    <s v="For the same reason as before, some of the graphs taper off slightly however the line of best fit for 9 is a curve."/>
+    <s v="6"/>
+    <n v="5"/>
+    <s v="line of best fit curves up above the x-axis and then curves back down below it"/>
+    <s v="5"/>
+    <s v="3"/>
+    <s v="The data seems a lot less clustered"/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="It is a lot more curved than the others"/>
+    <s v="5"/>
+    <n v="5"/>
+    <m/>
+    <s v="6"/>
+    <s v="3"/>
+    <m/>
+    <s v="7"/>
+    <s v="3"/>
+    <s v="data seems a lot more spreadout"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 4"/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="The line of best fit"/>
+    <s v="9"/>
+    <s v="4"/>
+    <m/>
+    <s v="6"/>
+    <s v="4"/>
+    <m/>
+    <s v="3"/>
+    <s v="2"/>
+    <m/>
+    <x v="0"/>
+    <n v="5"/>
+    <m/>
+    <s v="5"/>
+    <s v="4"/>
+    <m/>
+    <s v="6"/>
+    <s v="4"/>
+    <m/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 5"/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="More curvier"/>
+    <s v="9"/>
+    <n v="5"/>
+    <s v="More curvier "/>
+    <s v="6"/>
+    <n v="5"/>
+    <s v="Jagged"/>
+    <n v="0"/>
+    <n v="5"/>
+    <m/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="Big parabola "/>
+    <s v="5"/>
+    <n v="5"/>
+    <m/>
+    <s v="6"/>
+    <n v="5"/>
+    <m/>
+    <n v="0"/>
+    <n v="5"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 5"/>
+    <x v="0"/>
+    <s v="4"/>
+    <m/>
+    <s v="9"/>
+    <s v="4"/>
+    <m/>
+    <s v="7"/>
+    <s v="3"/>
+    <m/>
+    <s v="2"/>
+    <s v="3"/>
+    <m/>
+    <x v="0"/>
+    <s v="4"/>
+    <m/>
+    <s v="5"/>
+    <s v="3"/>
+    <m/>
+    <s v="6"/>
+    <s v="3"/>
+    <m/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 3"/>
+    <x v="0"/>
+    <s v="4"/>
+    <m/>
+    <s v="9"/>
+    <s v="4"/>
+    <m/>
+    <s v="4"/>
+    <s v="2"/>
+    <m/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+    <x v="0"/>
+    <s v="4"/>
+    <m/>
+    <s v="2"/>
+    <s v="2"/>
+    <m/>
+    <s v="6"/>
+    <s v="3"/>
+    <m/>
+    <n v="0"/>
+    <s v="2"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 4"/>
+    <x v="0"/>
+    <s v="4"/>
+    <s v="It is curvy"/>
+    <s v="9"/>
+    <s v="4"/>
+    <s v="It is more curvy "/>
+    <s v="4"/>
+    <s v="2"/>
+    <s v="It goes up"/>
+    <s v="2"/>
+    <n v="1"/>
+    <m/>
+    <x v="0"/>
+    <n v="5"/>
+    <m/>
+    <s v="5"/>
+    <s v="3"/>
+    <m/>
+    <s v="6"/>
+    <s v="2"/>
+    <m/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 4"/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="The only u-shaped red trend line"/>
+    <s v="9"/>
+    <n v="5"/>
+    <s v="the only n-shaped red trend line"/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="the only w-shaped red trend line"/>
+    <s v="5"/>
+    <s v="3"/>
+    <s v="kind of s-shaped red trend line, but also number 2 has w-shaped so unsure"/>
+    <s v="6"/>
+    <s v="4"/>
+    <s v="big upwards section at the end"/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 5"/>
+    <x v="0"/>
+    <s v="3"/>
+    <m/>
+    <s v="9"/>
+    <s v="2"/>
+    <m/>
+    <s v="5"/>
+    <s v="2"/>
+    <m/>
+    <n v="0"/>
+    <s v="2"/>
+    <m/>
+    <x v="0"/>
+    <s v="3"/>
+    <m/>
+    <s v="2"/>
+    <s v="2"/>
+    <m/>
+    <s v="6"/>
+    <s v="2"/>
+    <m/>
+    <n v="0"/>
+    <s v="2"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 5"/>
+    <x v="0"/>
+    <s v="4"/>
+    <s v="It's non-linear."/>
+    <s v="9"/>
+    <s v="4"/>
+    <s v="non-linear"/>
+    <n v="0"/>
+    <s v="2"/>
+    <m/>
+    <n v="0"/>
+    <s v="2"/>
+    <m/>
+    <x v="0"/>
+    <n v="5"/>
+    <m/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+    <s v="6"/>
+    <s v="2"/>
+    <m/>
+    <s v="7"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 5"/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="It has the largest movement away from the dotted line."/>
+    <s v="9"/>
+    <n v="5"/>
+    <s v="This red line has the largest difference from the dotted line."/>
+    <s v="4"/>
+    <n v="5"/>
+    <s v="It is the only plot that moves above the dotted line."/>
+    <s v="2"/>
+    <n v="5"/>
+    <s v="It has a large cluster of points below the line, where the others seeimgly have clusters of points randomly scattered."/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="It is a very significant parabolic curve, all the other curves are almosf straight."/>
+    <s v="5"/>
+    <n v="5"/>
+    <s v="Largest movement from a horizontal line, which the others seemingly follow."/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+    <s v="5"/>
+    <s v="2"/>
+    <s v="The most significant cluster at the top of graph."/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 3"/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="Looks like a curve while the rest are lines"/>
+    <s v="9"/>
+    <n v="5"/>
+    <s v="Curve and not line"/>
+    <s v="6"/>
+    <s v="3"/>
+    <s v="Looks a bit like a curve"/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="Curve"/>
+    <s v="2"/>
+    <s v="4"/>
+    <s v="Parabola "/>
+    <s v="6"/>
+    <s v="2"/>
+    <m/>
+    <s v="9"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="Year 4"/>
+    <x v="0"/>
+    <s v="2"/>
+    <s v="The other plots have roughly uniform distribution of points above and below the x axis, while 8 has more above at the extremes, and more below in the centre."/>
+    <s v="9"/>
+    <s v="2"/>
+    <s v="As with last time (but the opposite way round), the number of points below the axis spikes at the edges "/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+    <x v="0"/>
+    <s v="3"/>
+    <s v="Points seem to follow a fitted curve must more closely than any other plots"/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+    <s v="5"/>
+    <n v="1"/>
+    <s v="Wider spread of points at around 1.5"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 4"/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="It is quadratic. "/>
+    <s v="8"/>
+    <s v="4"/>
+    <s v="Quadratic"/>
+    <s v="4"/>
+    <s v="3"/>
+    <s v="Exponential, however 6 also looks like it stands out. "/>
+    <s v="5"/>
+    <s v="3"/>
+    <s v="Slight fanning towards the right. "/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="Clear quadratic trend. "/>
+    <s v="4"/>
+    <s v="3"/>
+    <s v="Has the least trend. "/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="Year 4"/>
+    <x v="0"/>
+    <s v="3"/>
+    <s v="It's a curve rather than a line"/>
+    <s v="6"/>
+    <s v="3"/>
+    <s v="the line seems more random"/>
+    <s v="4"/>
+    <s v="3"/>
+    <s v="It's the only one with a vaguelty upward trajectory"/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+    <x v="0"/>
+    <s v="2"/>
+    <s v="The beginning and end of the line are the most extreme"/>
+    <s v="2"/>
+    <n v="1"/>
+    <s v="There is a row of dots along the top that is more consistant than the rest"/>
+    <s v="7"/>
+    <n v="1"/>
+    <s v="7 has the smoothest line"/>
+    <s v="5"/>
+    <n v="1"/>
+    <s v="The line along the top is the most consistant"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 5"/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="The line of best fit is not linear"/>
+    <s v="9"/>
+    <s v="4"/>
+    <s v="This was the plot with the least linear line of best fit"/>
+    <s v="3"/>
+    <s v="2"/>
+    <s v="The data seems a little more spread out"/>
+    <s v="3"/>
+    <s v="2"/>
+    <s v="The data is slighty more spread out"/>
+    <x v="0"/>
+    <s v="3"/>
+    <s v="The line of best fit is not horizontal"/>
+    <s v="5"/>
+    <s v="2"/>
+    <s v="The line of best fit, seems the least horizontal"/>
+    <s v="6"/>
+    <n v="1"/>
+    <s v="The data seems the most spread out"/>
+    <s v="5"/>
+    <s v="3"/>
+    <s v="This data seems to be the most linear"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <x v="0"/>
+    <s v="4"/>
+    <s v="With the other plots the red line appears to be linear, while in the case of the chosen QQ-plot the red linear looks quadratic."/>
+    <s v="9"/>
+    <s v="3"/>
+    <s v="Weighting on the tails appear to be different compared to all the other plots. "/>
+    <s v="5"/>
+    <s v="3"/>
+    <s v="Has a weird curve around the centre of mass. "/>
+    <s v="6"/>
+    <s v="2"/>
+    <s v="How far away the points are on the upper right hand side."/>
+    <x v="0"/>
+    <s v="4"/>
+    <m/>
+    <s v="5"/>
+    <s v="3"/>
+    <m/>
+    <s v="6"/>
+    <s v="4"/>
+    <m/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 5"/>
+    <x v="0"/>
+    <s v="4"/>
+    <s v="The red curve stands out."/>
+    <s v="9"/>
+    <n v="5"/>
+    <s v="The red curve is the only one that makes a cone."/>
+    <s v="6"/>
+    <s v="2"/>
+    <s v="The red curve has more of a bump in the middle of the plot compared to the others."/>
+    <n v="0"/>
+    <s v="4"/>
+    <m/>
+    <x v="0"/>
+    <s v="3"/>
+    <m/>
+    <s v="5"/>
+    <s v="2"/>
+    <s v="The red curve seems to not fit the same pattern as the rest."/>
+    <s v="8"/>
+    <s v="4"/>
+    <m/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <x v="0"/>
+    <s v="2"/>
+    <m/>
+    <s v="9"/>
+    <s v="2"/>
+    <m/>
+    <n v="0"/>
+    <s v="2"/>
+    <m/>
+    <n v="0"/>
+    <s v="2"/>
+    <m/>
+    <x v="0"/>
+    <s v="2"/>
+    <m/>
+    <s v="5"/>
+    <s v="2"/>
+    <m/>
+    <s v="6"/>
+    <s v="2"/>
+    <m/>
+    <n v="0"/>
+    <s v="2"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 4"/>
+    <x v="0"/>
+    <s v="2"/>
+    <m/>
+    <s v="9"/>
+    <s v="2"/>
+    <m/>
+    <s v="6"/>
+    <n v="1"/>
+    <m/>
+    <s v="2"/>
+    <n v="1"/>
+    <m/>
+    <x v="0"/>
+    <s v="2"/>
+    <m/>
+    <s v="5"/>
+    <s v="2"/>
+    <m/>
+    <s v="6"/>
+    <s v="2"/>
+    <m/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <x v="1"/>
+    <s v="4"/>
+    <m/>
+    <s v="9"/>
+    <n v="5"/>
+    <m/>
+    <s v="6"/>
+    <n v="5"/>
+    <m/>
+    <s v="5"/>
+    <n v="5"/>
+    <m/>
+    <x v="0"/>
+    <n v="5"/>
+    <m/>
+    <s v="5"/>
+    <n v="5"/>
+    <m/>
+    <s v="7"/>
+    <n v="5"/>
+    <m/>
+    <s v="4"/>
+    <n v="5"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 4"/>
+    <x v="0"/>
+    <s v="3"/>
+    <s v="curved red line"/>
+    <s v="9"/>
+    <s v="3"/>
+    <s v="curved red line"/>
+    <s v="6"/>
+    <s v="2"/>
+    <m/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+    <x v="0"/>
+    <s v="3"/>
+    <s v="curved red line "/>
+    <s v="5"/>
+    <s v="2"/>
+    <s v="red line"/>
+    <s v="6"/>
+    <n v="1"/>
+    <m/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <m/>
+    <x v="0"/>
+    <s v="3"/>
+    <m/>
+    <s v="9"/>
+    <s v="3"/>
+    <m/>
+    <s v="6"/>
+    <s v="3"/>
+    <m/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+    <x v="0"/>
+    <s v="3"/>
+    <m/>
+    <s v="5"/>
+    <s v="3"/>
+    <m/>
+    <s v="6"/>
+    <s v="3"/>
+    <m/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <m/>
+    <x v="0"/>
+    <n v="1"/>
+    <m/>
+    <s v="9"/>
+    <n v="1"/>
+    <m/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+    <x v="0"/>
+    <n v="1"/>
+    <m/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+    <s v="6"/>
+    <n v="1"/>
+    <m/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <m/>
+    <x v="0"/>
+    <s v="3"/>
+    <m/>
+    <s v="9"/>
+    <s v="3"/>
+    <m/>
+    <s v="6"/>
+    <s v="3"/>
+    <m/>
+    <n v="0"/>
+    <s v="2"/>
+    <m/>
+    <x v="0"/>
+    <s v="2"/>
+    <m/>
+    <s v="2"/>
+    <s v="2"/>
+    <m/>
+    <s v="6"/>
+    <s v="2"/>
+    <m/>
+    <n v="0"/>
+    <s v="2"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <m/>
+    <x v="0"/>
+    <n v="5"/>
+    <m/>
+    <s v="9"/>
+    <s v="4"/>
+    <m/>
+    <n v="0"/>
+    <s v="4"/>
+    <m/>
+    <n v="0"/>
+    <s v="4"/>
+    <m/>
+    <x v="0"/>
+    <n v="5"/>
+    <m/>
+    <s v="2"/>
+    <s v="3"/>
+    <m/>
+    <s v="6"/>
+    <s v="4"/>
+    <m/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <x v="0"/>
+    <n v="1"/>
+    <m/>
+    <s v="8"/>
+    <n v="1"/>
+    <m/>
+    <s v="6"/>
+    <n v="1"/>
+    <m/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+    <x v="0"/>
+    <n v="1"/>
+    <m/>
+    <s v="2"/>
+    <n v="1"/>
+    <m/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <m/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="having a strong trend of quadratic "/>
+    <s v="9"/>
+    <n v="5"/>
+    <s v="Same as the previous quesiton "/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="A strong trend "/>
+    <s v="5"/>
+    <s v="4"/>
+    <s v="It follows x^3 approximately "/>
+    <s v="6"/>
+    <s v="3"/>
+    <m/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 4"/>
+    <x v="0"/>
+    <s v="3"/>
+    <m/>
+    <s v="9"/>
+    <n v="1"/>
+    <m/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+    <s v="2"/>
+    <s v="2"/>
+    <m/>
+    <x v="0"/>
+    <s v="3"/>
+    <m/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 4"/>
+    <x v="2"/>
+    <s v="3"/>
+    <m/>
+    <n v="0"/>
+    <s v="2"/>
+    <m/>
+    <s v="9"/>
+    <s v="2"/>
+    <m/>
+    <s v="3"/>
+    <s v="2"/>
+    <m/>
+    <x v="1"/>
+    <s v="3"/>
+    <m/>
+    <s v="2"/>
+    <s v="3"/>
+    <m/>
+    <s v="5"/>
+    <s v="3"/>
+    <m/>
+    <s v="8"/>
+    <s v="3"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="Quadratic"/>
+    <s v="9"/>
+    <s v="4"/>
+    <s v="Quadratic"/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="Quadratic"/>
+    <s v="2"/>
+    <s v="4"/>
+    <s v="Quadratic"/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+    <n v="0"/>
+    <s v="2"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <x v="0"/>
+    <s v="3"/>
+    <m/>
+    <s v="9"/>
+    <s v="3"/>
+    <m/>
+    <s v="6"/>
+    <s v="2"/>
+    <m/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+    <x v="0"/>
+    <s v="3"/>
+    <m/>
+    <s v="5"/>
+    <s v="2"/>
+    <m/>
+    <s v="6"/>
+    <s v="2"/>
+    <m/>
+    <s v="9"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <x v="0"/>
+    <n v="5"/>
+    <m/>
+    <s v="9"/>
+    <n v="5"/>
+    <m/>
+    <s v="7"/>
+    <n v="5"/>
+    <m/>
+    <s v="2"/>
+    <s v="2"/>
+    <m/>
+    <x v="0"/>
+    <n v="5"/>
+    <m/>
+    <s v="5"/>
+    <s v="3"/>
+    <m/>
+    <s v="6"/>
+    <s v="4"/>
+    <m/>
+    <s v="3"/>
+    <s v="3"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <x v="0"/>
+    <s v="4"/>
+    <s v="red line not straight"/>
+    <s v="9"/>
+    <s v="3"/>
+    <m/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+    <s v="2"/>
+    <s v="3"/>
+    <m/>
+    <x v="0"/>
+    <s v="3"/>
+    <m/>
+    <s v="3"/>
+    <s v="3"/>
+    <s v="kinda fan out"/>
+    <n v="0"/>
+    <s v="2"/>
+    <m/>
+    <n v="0"/>
+    <s v="2"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 4"/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="It looks quadratic as opposed to linear "/>
+    <s v="9"/>
+    <s v="4"/>
+    <m/>
+    <s v="6"/>
+    <s v="2"/>
+    <m/>
+    <n v="0"/>
+    <s v="2"/>
+    <m/>
+    <x v="0"/>
+    <n v="5"/>
+    <m/>
+    <s v="5"/>
+    <s v="3"/>
+    <m/>
+    <s v="6"/>
+    <n v="1"/>
+    <m/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 4"/>
+    <x v="0"/>
+    <s v="3"/>
+    <s v="Fitted line has the most curvature"/>
+    <s v="9"/>
+    <s v="4"/>
+    <m/>
+    <s v="7"/>
+    <s v="2"/>
+    <s v="Curves up rather than down"/>
+    <n v="0"/>
+    <s v="4"/>
+    <m/>
+    <x v="0"/>
+    <s v="3"/>
+    <m/>
+    <s v="5"/>
+    <n v="1"/>
+    <m/>
+    <n v="0"/>
+    <s v="2"/>
+    <m/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="Points are following a pattern."/>
+    <s v="9"/>
+    <s v="4"/>
+    <m/>
+    <n v="0"/>
+    <s v="4"/>
+    <m/>
+    <n v="0"/>
+    <s v="4"/>
+    <m/>
+    <x v="0"/>
+    <s v="4"/>
+    <s v="The pattern is followed"/>
+    <n v="0"/>
+    <s v="4"/>
+    <m/>
+    <n v="0"/>
+    <s v="4"/>
+    <m/>
+    <n v="0"/>
+    <s v="4"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <x v="0"/>
+    <s v="3"/>
+    <s v="Trend in the residuals"/>
+    <s v="9"/>
+    <s v="3"/>
+    <s v="Trend in the residuals "/>
+    <s v="6"/>
+    <n v="1"/>
+    <m/>
+    <s v="8"/>
+    <s v="2"/>
+    <s v="There seems to be a greater number of negative residuals "/>
+    <x v="0"/>
+    <s v="3"/>
+    <s v="Clear trend in square root residuals"/>
+    <s v="2"/>
+    <s v="2"/>
+    <m/>
+    <s v="6"/>
+    <s v="2"/>
+    <m/>
+    <s v="5"/>
+    <s v="2"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <x v="0"/>
+    <s v="3"/>
+    <m/>
+    <s v="9"/>
+    <s v="3"/>
+    <m/>
+    <s v="4"/>
+    <s v="2"/>
+    <m/>
+    <s v="5"/>
+    <s v="2"/>
+    <m/>
+    <x v="0"/>
+    <s v="3"/>
+    <m/>
+    <s v="2"/>
+    <n v="1"/>
+    <m/>
+    <s v="6"/>
+    <n v="1"/>
+    <m/>
+    <n v="0"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="1"/>
+    <x v="1"/>
+    <m/>
+    <x v="0"/>
+    <s v="3"/>
+    <m/>
+    <s v="9"/>
+    <s v="3"/>
+    <m/>
+    <s v="6"/>
+    <s v="2"/>
+    <m/>
+    <s v="2"/>
+    <n v="1"/>
+    <m/>
+    <x v="0"/>
+    <s v="3"/>
+    <m/>
+    <s v="5"/>
+    <s v="2"/>
+    <m/>
+    <s v="6"/>
+    <s v="2"/>
+    <m/>
+    <s v="6"/>
+    <s v="2"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <m/>
+    <x v="0"/>
+    <s v="4"/>
+    <m/>
+    <s v="9"/>
+    <s v="4"/>
+    <m/>
+    <n v="0"/>
+    <n v="5"/>
+    <m/>
+    <n v="0"/>
+    <s v="4"/>
+    <m/>
+    <x v="0"/>
+    <s v="4"/>
+    <m/>
+    <s v="5"/>
+    <s v="4"/>
+    <m/>
+    <n v="0"/>
+    <s v="4"/>
+    <m/>
+    <n v="0"/>
+    <s v="4"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 4"/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="Seems like this one is quadratic, while others are linear"/>
+    <s v="9"/>
+    <n v="5"/>
+    <m/>
+    <s v="4"/>
+    <s v="4"/>
+    <m/>
+    <s v="5"/>
+    <s v="3"/>
+    <m/>
+    <x v="0"/>
+    <n v="5"/>
+    <m/>
+    <s v="5"/>
+    <n v="5"/>
+    <s v="This one seems like cubic"/>
+    <s v="6"/>
+    <n v="1"/>
+    <m/>
+    <s v="5"/>
+    <s v="3"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 5"/>
+    <x v="0"/>
+    <s v="3"/>
+    <s v="ContAiminated data "/>
+    <s v="9"/>
+    <s v="2"/>
+    <m/>
+    <s v="6"/>
+    <n v="1"/>
+    <m/>
+    <n v="0"/>
+    <s v="2"/>
+    <m/>
+    <x v="0"/>
+    <s v="3"/>
+    <m/>
+    <s v="5"/>
+    <s v="2"/>
+    <m/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+    <s v="4"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="1"/>
+    <m/>
+    <x v="0"/>
+    <s v="4"/>
+    <s v="Curved line rather than straight line for residuals vs fitted"/>
+    <s v="9"/>
+    <s v="4"/>
+    <s v="Tail ends both go in same direction unlike others for residuals vs fitted"/>
+    <s v="8"/>
+    <s v="2"/>
+    <s v="Only one that sticks to the same line?"/>
+    <n v="0"/>
+    <s v="2"/>
+    <s v="All seem similar in terms of residual vs fitted"/>
+    <x v="0"/>
+    <s v="4"/>
+    <s v="Follows a different trend to the rest for line of best fit"/>
+    <s v="5"/>
+    <s v="2"/>
+    <s v="Tail ends more pronounced compared to the rest?"/>
+    <s v="6"/>
+    <s v="2"/>
+    <s v="Bump goes up more closer in regards to line of best fit compared to rest of residuals vs fitted"/>
+    <n v="0"/>
+    <s v="3"/>
+    <s v="They all seem different but not to a great degree compared to another one"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 5"/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="It has a parabola shape instead of a straight line-ish shape"/>
+    <s v="9"/>
+    <s v="4"/>
+    <s v="It is not so evenly concentrated"/>
+    <s v="6"/>
+    <n v="1"/>
+    <m/>
+    <s v="2"/>
+    <s v="3"/>
+    <m/>
+    <x v="0"/>
+    <n v="5"/>
+    <m/>
+    <s v="5"/>
+    <n v="1"/>
+    <m/>
+    <s v="6"/>
+    <n v="1"/>
+    <m/>
+    <s v="8"/>
+    <n v="1"/>
+    <m/>
+  </r>
+  <r>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Year 5"/>
+    <x v="0"/>
+    <s v="4"/>
+    <s v="There seems to be a quadratic relationship in the residuals vs fitted plot in plot 8 indicating that the underlying relationship is in fact not linear"/>
+    <s v="9"/>
+    <n v="5"/>
+    <s v="Looks quadratic "/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+    <n v="0"/>
+    <s v="4"/>
+    <m/>
+    <x v="0"/>
+    <n v="5"/>
+    <s v="Looks like some x^4 shenanigans is going on here "/>
+    <s v="5"/>
+    <s v="4"/>
+    <s v="Line go cubic "/>
+    <n v="0"/>
+    <s v="3"/>
+    <m/>
+    <n v="0"/>
+    <n v="5"/>
+    <m/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{49140863-B148-48B0-8B18-3DFD0D63A5F0}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A4:B11" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+  <pivotFields count="27">
+    <pivotField axis="axisRow" dataField="1" showAll="0" sortType="descending">
+      <items count="3">
+        <item x="0"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="4">
+        <item h="1" x="1"/>
+        <item h="1" x="2"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
+      <items count="3">
+        <item h="1" x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="2">
+    <field x="1"/>
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="7">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="1">
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pageFields count="2">
+    <pageField fld="3" hier="-1"/>
+    <pageField fld="15" hier="-1"/>
+  </pageFields>
+  <dataFields count="1">
+    <dataField name="Count of Stats Y2" fld="0" subtotal="count" baseField="0" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AA58" totalsRowShown="0">
   <autoFilter ref="A1:AA58" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
@@ -1037,30 +2935,30 @@
     <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Stats Y2" dataDxfId="60"/>
     <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Level of study" dataDxfId="59"/>
     <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="Year of study" dataDxfId="58"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="LU1" dataDxfId="41"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="LU1_confidence" dataDxfId="57"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="LU1_comments" dataDxfId="56"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="LU2" dataDxfId="40"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="LU2_confidence" dataDxfId="55"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="LU2_comments" dataDxfId="54"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="LU3" dataDxfId="39"/>
-    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="LU3_confidence" dataDxfId="53"/>
-    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="LU3_comments" dataDxfId="52"/>
-    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="LU4" dataDxfId="38"/>
-    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="LU4_confidence" dataDxfId="51"/>
-    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="LU4_comments" dataDxfId="50"/>
-    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="LU5" dataDxfId="37"/>
-    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="LU5_confidence" dataDxfId="49"/>
-    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="LU5_comments" dataDxfId="48"/>
-    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="LU6" dataDxfId="36"/>
-    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="LU6_confidence" dataDxfId="47"/>
-    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="LU6_comments" dataDxfId="46"/>
-    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="LU7" dataDxfId="35"/>
-    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="LU7_confidence" dataDxfId="45"/>
-    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="LU7_comments" dataDxfId="44"/>
-    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="LU8" dataDxfId="34"/>
-    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="LU8_confidence" dataDxfId="43"/>
-    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="LU8_comments" dataDxfId="42"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0000-00000B000000}" name="LU1" dataDxfId="57"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="LU1_confidence" dataDxfId="56"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="LU1_comments" dataDxfId="55"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0000-00000E000000}" name="LU2" dataDxfId="54"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0000-00000F000000}" name="LU2_confidence" dataDxfId="53"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="LU2_comments" dataDxfId="52"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="LU3" dataDxfId="51"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="LU3_confidence" dataDxfId="50"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="LU3_comments" dataDxfId="49"/>
+    <tableColumn id="20" xr3:uid="{00000000-0010-0000-0000-000014000000}" name="LU4" dataDxfId="48"/>
+    <tableColumn id="21" xr3:uid="{00000000-0010-0000-0000-000015000000}" name="LU4_confidence" dataDxfId="47"/>
+    <tableColumn id="22" xr3:uid="{00000000-0010-0000-0000-000016000000}" name="LU4_comments" dataDxfId="46"/>
+    <tableColumn id="23" xr3:uid="{00000000-0010-0000-0000-000017000000}" name="LU5" dataDxfId="45"/>
+    <tableColumn id="24" xr3:uid="{00000000-0010-0000-0000-000018000000}" name="LU5_confidence" dataDxfId="44"/>
+    <tableColumn id="25" xr3:uid="{00000000-0010-0000-0000-000019000000}" name="LU5_comments" dataDxfId="43"/>
+    <tableColumn id="26" xr3:uid="{00000000-0010-0000-0000-00001A000000}" name="LU6" dataDxfId="42"/>
+    <tableColumn id="27" xr3:uid="{00000000-0010-0000-0000-00001B000000}" name="LU6_confidence" dataDxfId="41"/>
+    <tableColumn id="28" xr3:uid="{00000000-0010-0000-0000-00001C000000}" name="LU6_comments" dataDxfId="40"/>
+    <tableColumn id="29" xr3:uid="{00000000-0010-0000-0000-00001D000000}" name="LU7" dataDxfId="39"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="LU7_confidence" dataDxfId="38"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="LU7_comments" dataDxfId="37"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="LU8" dataDxfId="36"/>
+    <tableColumn id="33" xr3:uid="{00000000-0010-0000-0000-000021000000}" name="LU8_confidence" dataDxfId="35"/>
+    <tableColumn id="34" xr3:uid="{00000000-0010-0000-0000-000022000000}" name="LU8_comments" dataDxfId="34"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1408,8 +3306,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="X14" sqref="X14"/>
+    <sheetView topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F1" sqref="A1:AA58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10206,4 +12104,101 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30493275-168B-4CB5-9904-19906AC9AF6C}">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="5" t="s">
+        <v>224</v>
+      </c>
+      <c r="B1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="B4" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>176</v>
+      </c>
+      <c r="B5" s="8">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="8">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B7" s="8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="8">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="8">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="B11" s="8">
+        <v>55</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>